<commit_message>
Nuovo grafico curva di urgenza
</commit_message>
<xml_diff>
--- a/CurvaDiUrgenza.xlsx
+++ b/CurvaDiUrgenza.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Simone.Bertolini\Documents\GitHub\UsabilitaProject\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -13,10 +18,6 @@
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -62,6 +63,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -82,13 +86,26 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.8512580277772673E-2"/>
+          <c:y val="4.9276630130819489E-2"/>
+          <c:w val="0.86134389912183618"/>
+          <c:h val="0.69304152042663314"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Visibilità Stato</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -123,6 +140,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Match Sistema-Mondo Reale</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -157,6 +177,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>User Control</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -191,6 +214,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>Coerenza e Standard</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -225,6 +251,9 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>Prevenzione Errori</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575">
               <a:noFill/>
@@ -264,27 +293,46 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="42222720"/>
-        <c:axId val="232148352"/>
+        <c:axId val="511716576"/>
+        <c:axId val="511711480"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="42222720"/>
+        <c:axId val="511716576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Impatto</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="232148352"/>
+        <c:crossAx val="511711480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="232148352"/>
+        <c:axId val="511711480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -299,11 +347,30 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Frequenza</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="42222720"/>
+        <c:crossAx val="511716576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -316,8 +383,17 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
+      <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="2.8192067497917011E-2"/>
+          <c:y val="0.88038121873340858"/>
+          <c:w val="0.92750565911124838"/>
+          <c:h val="0.11961878126659137"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -337,16 +413,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>485775</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>124483</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>168822</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>578069</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>26276</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -372,37 +448,41 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.31695</cdr:x>
-      <cdr:y>0.46962</cdr:y>
+      <cdr:x>0.07431</cdr:x>
+      <cdr:y>0.16503</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.44378</cdr:x>
-      <cdr:y>0.47179</cdr:y>
+      <cdr:x>0.23339</cdr:x>
+      <cdr:y>0.16503</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="5" name="Connettore 1 4"/>
+        <cdr:cNvPr id="13" name="Connettore 1 12"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="1443037" y="1288256"/>
-          <a:ext cx="577453" cy="5953"/>
+          <a:off x="351489" y="573785"/>
+          <a:ext cx="752425" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -412,37 +492,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.44116</cdr:x>
-      <cdr:y>0.60995</cdr:y>
+      <cdr:x>0.80647</cdr:x>
+      <cdr:y>0.62699</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.57241</cdr:x>
-      <cdr:y>0.60995</cdr:y>
+      <cdr:x>0.80647</cdr:x>
+      <cdr:y>0.75817</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="6" name="Connettore 1 5"/>
+        <cdr:cNvPr id="14" name="Connettore 1 13"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2011826" y="1673226"/>
-          <a:ext cx="598536" cy="0"/>
+          <a:off x="3814600" y="2180000"/>
+          <a:ext cx="0" cy="456126"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -452,37 +536,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.57322</cdr:x>
-      <cdr:y>0.7435</cdr:y>
+      <cdr:x>0.65809</cdr:x>
+      <cdr:y>0.62833</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.69773</cdr:x>
-      <cdr:y>0.74523</cdr:y>
+      <cdr:x>0.80696</cdr:x>
+      <cdr:y>0.62833</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="7" name="Connettore 1 6"/>
+        <cdr:cNvPr id="15" name="Connettore 1 14"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="2609850" y="2039572"/>
-          <a:ext cx="566900" cy="4731"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3112757" y="2184679"/>
+          <a:ext cx="704140" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -492,37 +580,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.31564</cdr:x>
-      <cdr:y>0.32422</cdr:y>
+      <cdr:x>0.51684</cdr:x>
+      <cdr:y>0.51286</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.31695</cdr:x>
-      <cdr:y>0.47179</cdr:y>
+      <cdr:x>0.66391</cdr:x>
+      <cdr:y>0.51286</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="8" name="Connettore 1 7"/>
+        <cdr:cNvPr id="16" name="Connettore 1 15"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
-          <a:off x="1437084" y="889397"/>
-          <a:ext cx="5953" cy="404812"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2444658" y="1783174"/>
+          <a:ext cx="695635" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -532,37 +624,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.18589</cdr:x>
-      <cdr:y>0.19017</cdr:y>
+      <cdr:x>0.37421</cdr:x>
+      <cdr:y>0.3959</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.18589</cdr:x>
-      <cdr:y>0.32906</cdr:y>
+      <cdr:x>0.5167</cdr:x>
+      <cdr:y>0.3959</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="11" name="Connettore 1 10"/>
+        <cdr:cNvPr id="18" name="Connettore 1 17"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="847726" y="521678"/>
-          <a:ext cx="0" cy="381000"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1769988" y="1376513"/>
+          <a:ext cx="673995" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -572,37 +668,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.0429</cdr:x>
-      <cdr:y>0.19097</cdr:y>
+      <cdr:x>0.2274</cdr:x>
+      <cdr:y>0.28083</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.18702</cdr:x>
-      <cdr:y>0.19097</cdr:y>
+      <cdr:x>0.37504</cdr:x>
+      <cdr:y>0.28083</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="3" name="Connettore 1 2"/>
+        <cdr:cNvPr id="20" name="Connettore 1 19"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="195629" y="523875"/>
-          <a:ext cx="657249" cy="1"/>
+          <a:off x="1075614" y="976421"/>
+          <a:ext cx="698334" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -612,37 +712,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.44104</cdr:x>
-      <cdr:y>0.46457</cdr:y>
+      <cdr:x>0.66095</cdr:x>
+      <cdr:y>0.51381</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.44296</cdr:x>
-      <cdr:y>0.61485</cdr:y>
+      <cdr:x>0.66095</cdr:x>
+      <cdr:y>0.62781</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="12" name="Connettore 1 11"/>
+        <cdr:cNvPr id="21" name="Connettore 1 20"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
-          <a:off x="2011265" y="1274398"/>
-          <a:ext cx="8767" cy="412260"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="3126273" y="1786477"/>
+          <a:ext cx="0" cy="396391"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -652,37 +756,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.69744</cdr:x>
-      <cdr:y>0.74306</cdr:y>
+      <cdr:x>0.51692</cdr:x>
+      <cdr:y>0.39414</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.69744</cdr:x>
-      <cdr:y>0.91016</cdr:y>
+      <cdr:x>0.51692</cdr:x>
+      <cdr:y>0.51256</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="19" name="Connettore 1 18"/>
+        <cdr:cNvPr id="22" name="Connettore 1 21"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="3175396" y="2038351"/>
-          <a:ext cx="0" cy="458390"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="2445035" y="1370420"/>
+          <a:ext cx="0" cy="411741"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -692,37 +800,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.18619</cdr:x>
-      <cdr:y>0.32639</cdr:y>
+      <cdr:x>0.3745</cdr:x>
+      <cdr:y>0.27867</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.31433</cdr:x>
-      <cdr:y>0.32639</cdr:y>
+      <cdr:x>0.3745</cdr:x>
+      <cdr:y>0.39354</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="4" name="Connettore 1 3"/>
+        <cdr:cNvPr id="23" name="Connettore 1 22"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="847725" y="895350"/>
-          <a:ext cx="583406" cy="0"/>
+          <a:off x="1771402" y="968916"/>
+          <a:ext cx="0" cy="399400"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -732,37 +844,41 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.57191</cdr:x>
-      <cdr:y>0.61068</cdr:y>
+      <cdr:x>0.22898</cdr:x>
+      <cdr:y>0.16682</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.57221</cdr:x>
-      <cdr:y>0.74573</cdr:y>
+      <cdr:x>0.22898</cdr:x>
+      <cdr:y>0.28207</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
-        <cdr:cNvPr id="17" name="Connettore 1 16"/>
+        <cdr:cNvPr id="24" name="Connettore 1 23"/>
         <cdr:cNvCxnSpPr/>
       </cdr:nvCxnSpPr>
       <cdr:spPr>
-        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipH="1" flipV="1">
-          <a:off x="2603896" y="1675209"/>
-          <a:ext cx="1331" cy="370468"/>
+        <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:off x="1083078" y="580040"/>
+          <a:ext cx="0" cy="400707"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
         </a:prstGeom>
-        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="12700"/>
+        <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
       </cdr:spPr>
       <cdr:style>
         <a:lnRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="1">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:lnRef>
         <a:fillRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:fillRef>
         <a:effectRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="0">
-          <a:schemeClr val="dk1"/>
+          <a:schemeClr val="accent1"/>
         </a:effectRef>
         <a:fontRef xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" idx="minor">
           <a:schemeClr val="tx1"/>
@@ -816,7 +932,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -851,7 +967,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1063,7 +1179,7 @@
   <dimension ref="A6:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>